<commit_message>
Metrics: Fix StdDev test tool.
</commit_message>
<xml_diff>
--- a/Metrics/Materials/StdDev Test Tool.xlsx
+++ b/Metrics/Materials/StdDev Test Tool.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Tracked Values</t>
   </si>
@@ -33,6 +33,15 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Max</t>
   </si>
 </sst>
 </file>
@@ -399,20 +408,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{596B173E-002B-4BE3-A095-A6805C061A89}">
-  <dimension ref="B2:D9"/>
+  <dimension ref="B2:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="13.5859375" customWidth="1"/>
-    <col min="3" max="3" width="29.64453125" customWidth="1"/>
-    <col min="4" max="4" width="40.8203125" customWidth="1"/>
+    <col min="3" max="6" width="34.5859375" customWidth="1"/>
+    <col min="7" max="7" width="20.1171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -422,45 +431,72 @@
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.5">
       <c r="C3" s="1">
         <f>_xlfn.STDEV.P(B:B)</f>
-        <v>0.44768152742770162</v>
+        <v>0.11180339887498954</v>
       </c>
       <c r="D3" s="1">
         <f>SUM(B:B)</f>
-        <v>1.4100000000000001</v>
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <f>MIN(B:B)</f>
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="1">
+        <f>MAX(B:B)</f>
+        <v>0.4</v>
+      </c>
+      <c r="G3">
+        <f>COUNT(B:B)</f>
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B4">
+        <v>0.1</v>
+      </c>
       <c r="C4" s="2">
         <f>C3</f>
-        <v>0.44768152742770162</v>
+        <v>0.11180339887498954</v>
       </c>
       <c r="D4" s="2">
         <f>D3</f>
-        <v>1.4100000000000001</v>
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <f>E3</f>
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="2">
+        <f>F3</f>
+        <v>0.4</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.5">
+      <c r="B5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B6">
-        <v>0.17</v>
+        <v>0.3</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B7">
-        <v>0.32</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B8">
-        <v>-0.15</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.5">
-      <c r="B9">
-        <v>1.07</v>
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Metrics: Even faster aggregators (work in progress, almost done, needs cleanup).
</commit_message>
<xml_diff>
--- a/Metrics/Materials/StdDev Test Tool.xlsx
+++ b/Metrics/Materials/StdDev Test Tool.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="17327" windowHeight="9360" xr2:uid="{2F59221E-A1B3-4271-9AF5-54C31D4D8A58}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Measurement" sheetId="1" r:id="rId1"/>
+    <sheet name="Accumulator" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Tracked Values</t>
   </si>
@@ -42,6 +43,15 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>Running Sum</t>
+  </si>
+  <si>
+    <t>Running Min</t>
+  </si>
+  <si>
+    <t>Running Max</t>
   </si>
 </sst>
 </file>
@@ -89,11 +99,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -411,7 +422,7 @@
   <dimension ref="B2:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -444,19 +455,19 @@
     <row r="3" spans="2:7" x14ac:dyDescent="0.5">
       <c r="C3" s="1">
         <f>_xlfn.STDEV.P(B:B)</f>
-        <v>0.11180339887498954</v>
+        <v>1.1180339887498949</v>
       </c>
       <c r="D3" s="1">
         <f>SUM(B:B)</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1">
         <f>MIN(B:B)</f>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1">
         <f>MAX(B:B)</f>
-        <v>0.4</v>
+        <v>4</v>
       </c>
       <c r="G3">
         <f>COUNT(B:B)</f>
@@ -465,42 +476,499 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B4">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2">
         <f>C3</f>
-        <v>0.11180339887498954</v>
+        <v>1.1180339887498949</v>
       </c>
       <c r="D4" s="2">
         <f>D3</f>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2">
         <f>E3</f>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="F4" s="2">
         <f>F3</f>
-        <v>0.4</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B5">
-        <v>0.2</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B6">
-        <v>0.3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.5">
       <c r="B7">
-        <v>0.4</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95FB7491-5675-43C4-A602-2B3AC714B245}">
+  <dimension ref="B2:E30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="2" max="2" width="16.17578125" customWidth="1"/>
+    <col min="3" max="4" width="23.29296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.9375" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="B3">
+        <v>0.4</v>
+      </c>
+      <c r="C3" s="2">
+        <f>SUM(B$3:B3)</f>
+        <v>0.4</v>
+      </c>
+      <c r="D3" s="2">
+        <f>MIN(C$3:C3)</f>
+        <v>0.4</v>
+      </c>
+      <c r="E3" s="2">
+        <f>MAX(C$3:C3)</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2">
+        <f>SUM(B$3:B4)</f>
+        <v>2.4</v>
+      </c>
+      <c r="D4" s="2">
+        <f>MIN(C$3:C4)</f>
+        <v>0.4</v>
+      </c>
+      <c r="E4" s="2">
+        <f>MAX(C$3:C4)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="B5">
+        <v>-2</v>
+      </c>
+      <c r="C5" s="2">
+        <f>SUM(B$3:B5)</f>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="D5" s="2">
+        <f>MIN(C$3:C5)</f>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="E5" s="2">
+        <f>MAX(C$3:C5)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="B6">
+        <v>0.17</v>
+      </c>
+      <c r="C6" s="2">
+        <f>SUM(B$3:B6)</f>
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D6" s="2">
+        <f>MIN(C$3:C6)</f>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="E6" s="2">
+        <f>MAX(C$3:C6)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="B7">
+        <v>0.32</v>
+      </c>
+      <c r="C7" s="2">
+        <f>SUM(B$3:B7)</f>
+        <v>0.8899999999999999</v>
+      </c>
+      <c r="D7" s="2">
+        <f>MIN(C$3:C7)</f>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="E7" s="2">
+        <f>MAX(C$3:C7)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="B8">
+        <v>-0.15</v>
+      </c>
+      <c r="C8" s="2">
+        <f>SUM(B$3:B8)</f>
+        <v>0.73999999999999988</v>
+      </c>
+      <c r="D8" s="2">
+        <f>MIN(C$3:C8)</f>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="E8" s="2">
+        <f>MAX(C$3:C8)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="B9">
+        <v>1.07</v>
+      </c>
+      <c r="C9" s="2">
+        <f>SUM(B$3:B9)</f>
+        <v>1.81</v>
+      </c>
+      <c r="D9" s="2">
+        <f>MIN(C$3:C9)</f>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="E9" s="2">
+        <f>MAX(C$3:C9)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <f>SUM(B$3:B10)</f>
+        <v>1.81</v>
+      </c>
+      <c r="D10" s="2">
+        <f>MIN(C$3:C10)</f>
+        <v>0.39999999999999991</v>
+      </c>
+      <c r="E10" s="2">
+        <f>MAX(C$3:C10)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="B11">
+        <v>-10</v>
+      </c>
+      <c r="C11" s="2">
+        <f>SUM(B$3:B11)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D11" s="2">
+        <f>MIN(C$3:C11)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E11" s="2">
+        <f>MAX(C$3:C11)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="C12" s="2">
+        <f>SUM(B$3:B12)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D12" s="2">
+        <f>MIN(C$3:C12)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E12" s="2">
+        <f>MAX(C$3:C12)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="C13" s="2">
+        <f>SUM(B$3:B13)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D13" s="2">
+        <f>MIN(C$3:C13)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E13" s="2">
+        <f>MAX(C$3:C13)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="C14" s="2">
+        <f>SUM(B$3:B14)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D14" s="2">
+        <f>MIN(C$3:C14)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E14" s="2">
+        <f>MAX(C$3:C14)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="C15" s="2">
+        <f>SUM(B$3:B15)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D15" s="2">
+        <f>MIN(C$3:C15)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E15" s="2">
+        <f>MAX(C$3:C15)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.5">
+      <c r="C16" s="2">
+        <f>SUM(B$3:B16)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D16" s="2">
+        <f>MIN(C$3:C16)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E16" s="2">
+        <f>MAX(C$3:C16)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.5">
+      <c r="C17" s="2">
+        <f>SUM(B$3:B17)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D17" s="2">
+        <f>MIN(C$3:C17)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E17" s="2">
+        <f>MAX(C$3:C17)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.5">
+      <c r="C18" s="2">
+        <f>SUM(B$3:B18)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D18" s="2">
+        <f>MIN(C$3:C18)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E18" s="2">
+        <f>MAX(C$3:C18)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.5">
+      <c r="C19" s="2">
+        <f>SUM(B$3:B19)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D19" s="2">
+        <f>MIN(C$3:C19)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E19" s="2">
+        <f>MAX(C$3:C19)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.5">
+      <c r="C20" s="2">
+        <f>SUM(B$3:B20)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D20" s="2">
+        <f>MIN(C$3:C20)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E20" s="2">
+        <f>MAX(C$3:C20)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.5">
+      <c r="C21" s="2">
+        <f>SUM(B$3:B21)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D21" s="2">
+        <f>MIN(C$3:C21)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E21" s="2">
+        <f>MAX(C$3:C21)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.5">
+      <c r="C22" s="2">
+        <f>SUM(B$3:B22)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D22" s="2">
+        <f>MIN(C$3:C22)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E22" s="2">
+        <f>MAX(C$3:C22)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.5">
+      <c r="C23" s="2">
+        <f>SUM(B$3:B23)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D23" s="2">
+        <f>MIN(C$3:C23)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E23" s="2">
+        <f>MAX(C$3:C23)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.5">
+      <c r="C24" s="2">
+        <f>SUM(B$3:B24)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D24" s="2">
+        <f>MIN(C$3:C24)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E24" s="2">
+        <f>MAX(C$3:C24)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.5">
+      <c r="C25" s="2">
+        <f>SUM(B$3:B25)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D25" s="2">
+        <f>MIN(C$3:C25)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E25" s="2">
+        <f>MAX(C$3:C25)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.5">
+      <c r="C26" s="2">
+        <f>SUM(B$3:B26)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D26" s="2">
+        <f>MIN(C$3:C26)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E26" s="2">
+        <f>MAX(C$3:C26)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.5">
+      <c r="C27" s="2">
+        <f>SUM(B$3:B27)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D27" s="2">
+        <f>MIN(C$3:C27)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E27" s="2">
+        <f>MAX(C$3:C27)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.5">
+      <c r="C28" s="2">
+        <f>SUM(B$3:B28)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D28" s="2">
+        <f>MIN(C$3:C28)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E28" s="2">
+        <f>MAX(C$3:C28)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.5">
+      <c r="C29" s="2">
+        <f>SUM(B$3:B29)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D29" s="2">
+        <f>MIN(C$3:C29)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E29" s="2">
+        <f>MAX(C$3:C29)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.5">
+      <c r="C30" s="2">
+        <f>SUM(B$3:B30)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="D30" s="2">
+        <f>MIN(C$3:C30)</f>
+        <v>-8.19</v>
+      </c>
+      <c r="E30" s="2">
+        <f>MAX(C$3:C30)</f>
+        <v>2.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C4:C6" formulaRange="1"/>
+  </ignoredErrors>
+</worksheet>
 </file>
</xml_diff>